<commit_message>
cleaning anynet related files
</commit_message>
<xml_diff>
--- a/Extras/Comparison.xlsx
+++ b/Extras/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tracks\CS4\graduation project\Implemented papers\Stereo-3D-Detection\Extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E529A64-BC2C-4F07-A318-9DC29848A499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1138F5AF-485D-4E0F-BB13-74EC9C55F196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD177DEC-EEDB-4228-BD18-6B038B114584}"/>
   </bookViews>
@@ -293,6 +293,12 @@
     <xf numFmtId="10" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -309,12 +315,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,12 +634,12 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="9" customWidth="1"/>
     <col min="2" max="17" width="10.5546875" style="1" customWidth="1"/>
     <col min="18" max="19" width="11.33203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="32.5546875" style="1" customWidth="1"/>
@@ -647,54 +647,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="29.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="16" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="14" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -749,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -802,7 +802,7 @@
         <v>0.29720000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
@@ -855,219 +855,219 @@
         <v>0.12265</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="10" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.11599</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.5989999999999993E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.568E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.14405999999999999</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.12374</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8.2860000000000003E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>7.739E-2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0.16388</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0.14266999999999999</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0.11509</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0.10673000000000001</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.16797999999999999</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0.14604</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0.11625000000000001</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0.10879999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="3">
         <v>0.15559999999999999</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="3">
         <v>0.11269999999999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="3">
         <v>7.4300000000000005E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="3">
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>0.14779999999999999</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="5">
         <v>9.7409999999999997E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H7" s="5">
         <v>6.7989999999999995E-2</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I7" s="5">
         <v>6.0920000000000002E-2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J7" s="13">
         <v>0.20064000000000001</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K7" s="13">
         <v>0.15462999999999999</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L7" s="13">
         <v>0.12407</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M7" s="13">
         <v>0.11728</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N7" s="12">
         <v>0.20752999999999999</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O7" s="12">
         <v>0.15875</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P7" s="12">
         <v>0.12484000000000001</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q7" s="12">
         <v>0.11816</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    <row r="8" spans="1:17" s="10" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.12101000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9.8419999999999994E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>7.1179999999999993E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5.9549999999999999E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.13517999999999999</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.11446000000000001</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.8060000000000004E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>6.9220000000000004E-2</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.15808</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0.13927999999999999</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0.11479</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0.10247000000000001</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.16113</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0.14187</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0.11514000000000001</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>0.10348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B9" s="3">
         <v>0.14584</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" s="3">
         <v>0.1007</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D9" s="3">
         <v>7.0739999999999997E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E9" s="3">
         <v>6.7970000000000003E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F9" s="5">
         <v>0.16391</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G9" s="5">
         <v>0.10929999999999999</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H9" s="5">
         <v>7.281E-2</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I9" s="5">
         <v>6.9610000000000005E-2</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J9" s="13">
         <v>0.17130000000000001</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K9" s="13">
         <v>0.1323</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L9" s="13">
         <v>0.10630000000000001</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M9" s="13">
         <v>9.9299999999999999E-2</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N9" s="12">
         <v>0.17788000000000001</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O9" s="12">
         <v>0.13633999999999999</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P9" s="12">
         <v>0.10767</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q9" s="12">
         <v>0.10099</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.11599</v>
-      </c>
-      <c r="C8" s="3">
-        <v>9.3600000000000003E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.5989999999999993E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>5.568E-2</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.14405999999999999</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.12374</v>
-      </c>
-      <c r="H8" s="5">
-        <v>8.2860000000000003E-2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>7.739E-2</v>
-      </c>
-      <c r="J8" s="13">
-        <v>0.16388</v>
-      </c>
-      <c r="K8" s="13">
-        <v>0.14266999999999999</v>
-      </c>
-      <c r="L8" s="13">
-        <v>0.11509</v>
-      </c>
-      <c r="M8" s="13">
-        <v>0.10673000000000001</v>
-      </c>
-      <c r="N8" s="12">
-        <v>0.16797999999999999</v>
-      </c>
-      <c r="O8" s="12">
-        <v>0.14604</v>
-      </c>
-      <c r="P8" s="12">
-        <v>0.11625000000000001</v>
-      </c>
-      <c r="Q8" s="12">
-        <v>0.10879999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.12101000000000001</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9.8419999999999994E-2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7.1179999999999993E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5.9549999999999999E-2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.13517999999999999</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.11446000000000001</v>
-      </c>
-      <c r="H9" s="5">
-        <v>7.8060000000000004E-2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>6.9220000000000004E-2</v>
-      </c>
-      <c r="J9" s="13">
-        <v>0.15808</v>
-      </c>
-      <c r="K9" s="13">
-        <v>0.13927999999999999</v>
-      </c>
-      <c r="L9" s="13">
-        <v>0.11479</v>
-      </c>
-      <c r="M9" s="13">
-        <v>0.10247000000000001</v>
-      </c>
-      <c r="N9" s="12">
-        <v>0.16113</v>
-      </c>
-      <c r="O9" s="12">
-        <v>0.14187</v>
-      </c>
-      <c r="P9" s="12">
-        <v>0.11514000000000001</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>0.10348</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="10" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1127,17 +1127,17 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
@@ -1146,17 +1146,17 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
@@ -1165,17 +1165,17 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
     </row>
     <row r="14" spans="1:17" s="10" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>

</xml_diff>